<commit_message>
Phones with PhoneGroup done
</commit_message>
<xml_diff>
--- a/public/uploads/MobileNumber.xlsx
+++ b/public/uploads/MobileNumber.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31708B76-EC1D-4454-B72D-9630DD8EE4BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D6736A-2078-4078-99CA-8F60109D6960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Phone</t>
+    <t>number</t>
   </si>
   <si>
     <t>01833184046</t>
   </si>
   <si>
-    <t>01833184045</t>
+    <t>01833184048</t>
+  </si>
+  <si>
+    <t>01833184049</t>
   </si>
 </sst>
 </file>
@@ -347,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,6 +376,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>